<commit_message>
dev-197 - fixed upload demand if shop code is numeric
</commit_message>
<xml_diff>
--- a/etc/scripts/demand_shops.xlsx
+++ b/etc/scripts/demand_shops.xlsx
@@ -25,10 +25,10 @@
     <t>Значение</t>
   </si>
   <si>
-    <t>adcd</t>
+    <t>0123</t>
   </si>
   <si>
-    <t>adce</t>
+    <t>122</t>
   </si>
 </sst>
 </file>
@@ -36,10 +36,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -65,68 +65,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -140,9 +81,106 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -155,44 +193,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -209,181 +209,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -397,21 +397,25 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -447,6 +451,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -466,170 +479,157 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -642,8 +642,9 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -995,8 +996,8 @@
   <sheetPr/>
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="15" outlineLevelCol="2"/>
@@ -1017,10 +1018,10 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
         <v>43951.4166666667</v>
       </c>
       <c r="C2">
@@ -1028,10 +1029,10 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
         <v>43951.5</v>
       </c>
       <c r="C3">
@@ -1039,10 +1040,10 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
         <v>43951.5416666667</v>
       </c>
       <c r="C4">
@@ -1050,10 +1051,10 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
         <v>43951.5833333333</v>
       </c>
       <c r="C5">
@@ -1061,10 +1062,10 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2">
         <v>43951.625</v>
       </c>
       <c r="C6">
@@ -1072,10 +1073,10 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2">
         <v>43951.6666666667</v>
       </c>
       <c r="C7">
@@ -1083,10 +1084,10 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2">
         <v>43951.7083333333</v>
       </c>
       <c r="C8">
@@ -1094,10 +1095,10 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="2">
         <v>43951.75</v>
       </c>
       <c r="C9">
@@ -1105,10 +1106,10 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1">
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="2">
         <v>43951.7916666667</v>
       </c>
       <c r="C10">
@@ -1116,10 +1117,10 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="1">
+      <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2">
         <v>43951.8333333333</v>
       </c>
       <c r="C11">
@@ -1127,10 +1128,10 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="1">
+      <c r="A12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2">
         <f>B2+1</f>
         <v>43952.4166666667</v>
       </c>
@@ -1139,10 +1140,10 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="1">
+      <c r="A13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2">
         <f t="shared" ref="B13:B21" si="0">B3+1</f>
         <v>43952.5</v>
       </c>
@@ -1151,10 +1152,10 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="1">
+      <c r="A14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2">
         <f t="shared" si="0"/>
         <v>43952.5416666667</v>
       </c>
@@ -1163,10 +1164,10 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="1">
+      <c r="A15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="2">
         <f t="shared" si="0"/>
         <v>43952.5833333333</v>
       </c>
@@ -1175,10 +1176,10 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="1">
+      <c r="A16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2">
         <f t="shared" si="0"/>
         <v>43952.625</v>
       </c>
@@ -1187,10 +1188,10 @@
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="1">
+      <c r="A17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2">
         <f t="shared" si="0"/>
         <v>43952.6666666667</v>
       </c>
@@ -1199,10 +1200,10 @@
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="1">
+      <c r="A18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="2">
         <f t="shared" si="0"/>
         <v>43952.7083333333</v>
       </c>
@@ -1211,10 +1212,10 @@
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="1">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2">
         <f t="shared" si="0"/>
         <v>43952.75</v>
       </c>
@@ -1223,10 +1224,10 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="1">
+      <c r="A20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="2">
         <f t="shared" si="0"/>
         <v>43952.7916666667</v>
       </c>
@@ -1235,10 +1236,10 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="1">
+      <c r="A21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2">
         <f t="shared" si="0"/>
         <v>43952.8333333333</v>
       </c>
@@ -1247,10 +1248,10 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="1">
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="2">
         <v>43951.4166666667</v>
       </c>
       <c r="C22">
@@ -1258,10 +1259,10 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="1">
+      <c r="A23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="2">
         <v>43951.5</v>
       </c>
       <c r="C23">
@@ -1269,10 +1270,10 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="1">
+      <c r="A24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="2">
         <v>43951.5416666667</v>
       </c>
       <c r="C24">
@@ -1280,10 +1281,10 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="1">
+      <c r="A25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="2">
         <v>43951.5833333333</v>
       </c>
       <c r="C25">
@@ -1291,10 +1292,10 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="1">
+      <c r="A26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="2">
         <v>43951.625</v>
       </c>
       <c r="C26">
@@ -1302,10 +1303,10 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="1">
+      <c r="A27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="2">
         <v>43951.6666666667</v>
       </c>
       <c r="C27">
@@ -1313,10 +1314,10 @@
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="1">
+      <c r="A28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="2">
         <v>43951.7083333333</v>
       </c>
       <c r="C28">
@@ -1324,10 +1325,10 @@
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29" s="1">
+      <c r="A29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="2">
         <v>43951.75</v>
       </c>
       <c r="C29">
@@ -1335,10 +1336,10 @@
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B30" s="1">
+      <c r="A30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="2">
         <v>43951.7916666667</v>
       </c>
       <c r="C30">
@@ -1346,10 +1347,10 @@
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="1">
+      <c r="A31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="2">
         <v>43951.8333333333</v>
       </c>
       <c r="C31">
@@ -1357,10 +1358,10 @@
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="1">
+      <c r="A32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="2">
         <f t="shared" ref="B32:B41" si="1">B22+1</f>
         <v>43952.4166666667</v>
       </c>
@@ -1369,10 +1370,10 @@
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" s="1">
+      <c r="A33" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="2">
         <f t="shared" si="1"/>
         <v>43952.5</v>
       </c>
@@ -1381,10 +1382,10 @@
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="1">
+      <c r="A34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="2">
         <f t="shared" si="1"/>
         <v>43952.5416666667</v>
       </c>
@@ -1393,10 +1394,10 @@
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="1">
+      <c r="A35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="2">
         <f t="shared" si="1"/>
         <v>43952.5833333333</v>
       </c>
@@ -1405,10 +1406,10 @@
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="1">
+      <c r="A36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="2">
         <f t="shared" si="1"/>
         <v>43952.625</v>
       </c>
@@ -1417,10 +1418,10 @@
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>4</v>
-      </c>
-      <c r="B37" s="1">
+      <c r="A37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="2">
         <f t="shared" si="1"/>
         <v>43952.6666666667</v>
       </c>
@@ -1429,10 +1430,10 @@
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" s="1">
+      <c r="A38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="2">
         <f t="shared" si="1"/>
         <v>43952.7083333333</v>
       </c>
@@ -1441,10 +1442,10 @@
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>4</v>
-      </c>
-      <c r="B39" s="1">
+      <c r="A39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="2">
         <f t="shared" si="1"/>
         <v>43952.75</v>
       </c>
@@ -1453,10 +1454,10 @@
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40" s="1">
+      <c r="A40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="2">
         <f t="shared" si="1"/>
         <v>43952.7916666667</v>
       </c>
@@ -1465,10 +1466,10 @@
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B41" s="1">
+      <c r="A41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="2">
         <f t="shared" si="1"/>
         <v>43952.8333333333</v>
       </c>

</xml_diff>